<commit_message>
finished negative reward chart making
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Discount Factor" sheetId="1" r:id="rId1"/>
     <sheet name="Step Cost" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Negative Reward" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Iterations</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Step Cost</t>
+  </si>
+  <si>
+    <t>Negative Reward</t>
   </si>
 </sst>
 </file>
@@ -1032,6 +1035,688 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iterations vs. Negative</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Reward (range: -10 to -100)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0466337569724882"/>
+          <c:y val="0.120634920634921"/>
+          <c:w val="0.884755608379141"/>
+          <c:h val="0.751463983668708"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Negative Reward'!$B$18:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-70.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-90.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Negative Reward'!$C$18:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2106322040"/>
+        <c:axId val="-2113082856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2106322040"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Negative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Reward</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2113082856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2113082856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="80.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00105374077976818"/>
+              <c:y val="0.414855319510331"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2106322040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iterations</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Negative Reward (range: -1 to -5)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0466337569724882"/>
+          <c:y val="0.120634920634921"/>
+          <c:w val="0.884755608379141"/>
+          <c:h val="0.751463983668708"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Negative Reward'!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Negative Reward'!$C$12:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2105917816"/>
+        <c:axId val="-2108116920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2105917816"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Negative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Reward</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2108116920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2108116920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00105374077976818"/>
+              <c:y val="0.414855319510331"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2105917816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iterations</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Negative Reward (range: 0 to -0.8)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0654882610680786"/>
+          <c:y val="0.148292682926829"/>
+          <c:w val="0.877543275045858"/>
+          <c:h val="0.694482555534217"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Negative Reward'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Negative Reward'!$C$6:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2105581624"/>
+        <c:axId val="-2096262312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2105581624"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Negative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Reward</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2096262312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2096262312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="80.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00101729399796541"/>
+              <c:y val="0.444944881889764"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2105581624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1145,6 +1830,101 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1759,6 +2539,283 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C14"/>
@@ -1875,7 +2932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
@@ -2062,13 +3119,197 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B5:C28"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="16">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="16">
+      <c r="B7" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="16">
+      <c r="B8" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="16">
+      <c r="B9" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="16">
+      <c r="B10" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="16">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="2:3" ht="16">
+      <c r="B12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="16">
+      <c r="B13" s="1">
+        <v>-2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="16">
+      <c r="B14" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="16">
+      <c r="B15" s="1">
+        <v>-4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="16">
+      <c r="B16" s="1">
+        <v>-5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="16">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" ht="16">
+      <c r="B18" s="1">
+        <v>-10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="16">
+      <c r="B19" s="1">
+        <v>-20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="16">
+      <c r="B20" s="1">
+        <v>-30</v>
+      </c>
+      <c r="C20" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="16">
+      <c r="B21" s="1">
+        <v>-40</v>
+      </c>
+      <c r="C21" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="16">
+      <c r="B22" s="1">
+        <v>-50</v>
+      </c>
+      <c r="C22" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="16">
+      <c r="B23" s="1">
+        <v>-60</v>
+      </c>
+      <c r="C23" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="16">
+      <c r="B24" s="1">
+        <v>-70</v>
+      </c>
+      <c r="C24" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="16">
+      <c r="B25" s="1">
+        <v>-80</v>
+      </c>
+      <c r="C25" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="16">
+      <c r="B26" s="1">
+        <v>-90</v>
+      </c>
+      <c r="C26" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="16">
+      <c r="B27" s="1">
+        <v>-100</v>
+      </c>
+      <c r="C27" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="16">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>